<commit_message>
Wyświetlanie rankingu i tras
</commit_message>
<xml_diff>
--- a/Projekt_zaliczeniowy/dataSheet/SZCZYTY.xlsx
+++ b/Projekt_zaliczeniowy/dataSheet/SZCZYTY.xlsx
@@ -5,17 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majka\OneDrive\Pulpit\AGH\5 semestr\Systemy Wspomagania Decyzji\ZZZ_copy\Projekt_zaliczeniowy_copy\dataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\STUDIA\Systemy wspomagania decyzji\Projekt\SWD\Projekt_zaliczeniowy\dataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C1193B-157A-42D3-9AB7-6C560A7B0F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19E798-9B3D-43EC-8478-D3621F92076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="16200" windowWidth="23175" windowHeight="8355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -70,126 +83,66 @@
     <t>Tatry Wysokie</t>
   </si>
   <si>
-    <t>Palenica Białczańska – Morskie Oko – Czarny Staw – Bula pod Rysami – Rysy</t>
-  </si>
-  <si>
     <t>Kasprowy Wierch</t>
   </si>
   <si>
     <t>Tatry Zachodnie</t>
   </si>
   <si>
-    <t>Kuźnice - leśniczówka, Myślenickie Turnie - Kasprowy Wierch</t>
-  </si>
-  <si>
     <t>Giewont</t>
   </si>
   <si>
-    <t>Kuźnice – Kalatówki – Hala Kondratowa – Kondracka Przełęcz – Wyżnia Kondracka Przełęcz – Giewont</t>
-  </si>
-  <si>
     <t>Lomnica</t>
   </si>
   <si>
-    <t>Tatrzańska Łomnica - Łomnicka Przełęcz - Łomnicka Kopa - Łomnica Staw</t>
-  </si>
-  <si>
     <t>Świnica</t>
   </si>
   <si>
-    <t>Kuźnice - Potok Bystra - Przełęcz między Kopami (Karczmisko) - Zielony Staw Gąsienicowy - Świnica</t>
-  </si>
-  <si>
     <t>Kościelec</t>
   </si>
   <si>
-    <t>Kuźnice – Boczań – Przełęcz między Kopami – Schronisko PTTK Murowaniec – Czarny Staw Gąsienicowy – Karb – Kościelec</t>
-  </si>
-  <si>
     <t>Lodowy Szczyt</t>
   </si>
   <si>
-    <t>Stary Smokowiec - Smokowieckie Siodełko - Rainerowa Chata - Schronisko Zamkowskie - Schronisko Tery'ego - Lodowy Szczyt</t>
-  </si>
-  <si>
     <t>Mały Gerlach</t>
   </si>
   <si>
-    <t xml:space="preserve">Tatrzańska Polanka - Śląski Dom - Mały Gerlach </t>
-  </si>
-  <si>
     <t>Durny Szczyt</t>
   </si>
   <si>
-    <t>Chata Teryego - Mała Durna Przełęcz - Mały Durny Sczyt - Durna Przełęcz - Durny Szczyt</t>
-  </si>
-  <si>
     <t>Krywań</t>
   </si>
   <si>
-    <t>Byvala Vazecka chata – Tri studnicky – Krivansky zlab – Maly Krywań – Krywań</t>
-  </si>
-  <si>
     <t>Dolina za Mnichem</t>
   </si>
   <si>
-    <t>Morskie Oko - Mnichowy Potok - Mnich</t>
-  </si>
-  <si>
     <t>Wołowiec</t>
   </si>
   <si>
-    <t>Siwa Polana - Wyżnia Brama Chochołowska - Schronisko na Polanie Chochołowskiej - Bobrowiecki Żleb - Grześ - Rakoń - Wołowiec</t>
-  </si>
-  <si>
     <t>Kozi Wierch</t>
   </si>
   <si>
-    <t>Palenica Białczańska – Wodogrzmoty Mickiewicza – Dolina Roztoki – Schronisko PTTK w Dolinie Pięciu Stawów Polskich – Kozi Wierch</t>
-  </si>
-  <si>
     <t>Sławkowski Szczyt</t>
   </si>
   <si>
-    <t>Stary Smokovec – Maksymilianka – Królewski Nos – Sławkowski Szczyt</t>
-  </si>
-  <si>
     <t>Wołoszyn</t>
   </si>
   <si>
-    <t>Dolina Filipka - Rusinowa Polana - Czerwone Brzeżki - Wołoszyn</t>
-  </si>
-  <si>
     <t>Bystra</t>
   </si>
   <si>
-    <t>Siwa Polana - Starorobociańska Dolina - Siwy Zwornik - Bystra</t>
-  </si>
-  <si>
     <t>Banówka</t>
   </si>
   <si>
-    <t>Schronisko Żarskie - Adamcula - Pod Hrubou kopou - Banówka</t>
-  </si>
-  <si>
     <t>Gęsia Szyja</t>
   </si>
   <si>
-    <t>Dolina Filipka - Rusinowa Polana - Gęsia Szyja</t>
-  </si>
-  <si>
     <t>Niżnie Rysy</t>
   </si>
   <si>
-    <t>Palenica Białczańska - Droga Oswalda Balzera, skrzyżowanie szlaków - Wodogrzmoty Mickiewicza - Wodogrzmoty Mickiewicza, odejście do Roztoki - Odejście na Kępę - Odejście na Szpiglasową Przełęcz -  Schronisko PTTK przy Morskim Oku - Morskie Oko - Morskie Oko, pod Czarnym Stawem - Czarny Staw Pod Rysami - Niższe Rysy</t>
-  </si>
-  <si>
     <t>Jagnięcy Szczyt</t>
   </si>
   <si>
-    <t>Biała Woda - Zimna Studnia - Schronisko nad Zielonym Stawem - Jagnięcy Szczyt</t>
-  </si>
-  <si>
     <t>Wysoka</t>
   </si>
   <si>
@@ -337,7 +290,67 @@
     <t>Babia góra Nowa</t>
   </si>
   <si>
-    <t>Zawoja - Babia Góra Nowa - Zawoja</t>
+    <t>Kuźnice-leśniczówka, Myślenickie Turnie-Kasprowy Wierch</t>
+  </si>
+  <si>
+    <t>Tatrzańska Łomnica-Łomnicka Przełęcz-Łomnicka Kopa-Łomnica Staw</t>
+  </si>
+  <si>
+    <t>Kuźnice-Potok Bystra-Przełęcz między Kopami (Karczmisko)-Zielony Staw Gąsienicowy-Świnica</t>
+  </si>
+  <si>
+    <t>Stary Smokowiec-Smokowieckie Siodełko-Rainerowa Chata-Schronisko Zamkowskie-Schronisko Tery'ego-Lodowy Szczyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatrzańska Polanka-Śląski Dom-Mały Gerlach </t>
+  </si>
+  <si>
+    <t>Chata Teryego-Mała Durna Przełęcz-Mały Durny Sczyt-Durna Przełęcz-Durny Szczyt</t>
+  </si>
+  <si>
+    <t>Morskie Oko-Mnichowy Potok-Mnich</t>
+  </si>
+  <si>
+    <t>Siwa Polana-Wyżnia Brama Chochołowska-Schronisko na Polanie Chochołowskiej-Bobrowiecki Żleb-Grześ-Rakoń-Wołowiec</t>
+  </si>
+  <si>
+    <t>Dolina Filipka-Rusinowa Polana-Czerwone Brzeżki-Wołoszyn</t>
+  </si>
+  <si>
+    <t>Siwa Polana-Starorobociańska Dolina-Siwy Zwornik-Bystra</t>
+  </si>
+  <si>
+    <t>Schronisko Żarskie-Adamcula-Pod Hrubou kopou-Banówka</t>
+  </si>
+  <si>
+    <t>Dolina Filipka-Rusinowa Polana-Gęsia Szyja</t>
+  </si>
+  <si>
+    <t>Biała Woda-Zimna Studnia-Schronisko nad Zielonym Stawem-Jagnięcy Szczyt</t>
+  </si>
+  <si>
+    <t>Zawoja-Babia Góra Nowa-Zawoja</t>
+  </si>
+  <si>
+    <t>Palenica Białczańska-Morskie Oko-Czarny Staw-Bula pod Rysami-Rysy</t>
+  </si>
+  <si>
+    <t>Kuźnice-Kalatówki-Hala Kondratowa-Kondracka Przełęcz-Wyżnia Kondracka Przełęcz-Giewont</t>
+  </si>
+  <si>
+    <t>Kuźnice-Boczań-Przełęcz między Kopami-Schronisko PTTK Murowaniec-Czarny Staw Gąsienicowy-Karb-Kościelec</t>
+  </si>
+  <si>
+    <t>Byvala Vazecka chata-Tri studnicky-Krivansky zlab-Maly Krywań-Krywań</t>
+  </si>
+  <si>
+    <t>Palenica Białczańska-Wodogrzmoty Mickiewicza-Dolina Roztoki-Schronisko PTTK w Dolinie Pięciu Stawów Polskich-Kozi Wierch</t>
+  </si>
+  <si>
+    <t>Stary Smokovec-Maksymilianka-Królewski Nos-Sławkowski Szczyt</t>
+  </si>
+  <si>
+    <t>Palenica Białczańska-Droga Oswalda Balzera-Wodogrzmoty Mickiewicza-Wodogrzmoty Mickiewicza-Odejście na Kępę-Odejście na Szpiglasową Przełęcz- PTTK Morskie Oko-Morskie Oko-Czarny Staw Pod Rysami-Niższe Rysy</t>
   </si>
 </sst>
 </file>
@@ -636,25 +649,25 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="47.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -697,7 +710,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3">
         <v>2501</v>
@@ -725,15 +738,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3">
         <v>1987</v>
@@ -761,15 +774,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3">
         <v>1895</v>
@@ -797,15 +810,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="D5" s="3">
         <v>2634</v>
@@ -833,15 +846,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D6" s="3">
         <v>2301</v>
@@ -870,15 +883,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="D7" s="3">
         <v>2155</v>
@@ -907,15 +920,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D8" s="3">
         <v>2627</v>
@@ -944,15 +957,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D9" s="3">
         <v>2601</v>
@@ -980,15 +993,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="D10" s="3">
         <v>2623</v>
@@ -1016,15 +1029,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="D11" s="3">
         <v>2495</v>
@@ -1052,15 +1065,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3">
         <v>1788</v>
@@ -1090,13 +1103,13 @@
     </row>
     <row r="13" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3">
         <v>2064</v>
@@ -1125,15 +1138,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="D14" s="3">
         <v>2291</v>
@@ -1161,15 +1174,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="D15" s="3">
         <v>2452</v>
@@ -1198,15 +1211,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="D16" s="3">
         <v>2155</v>
@@ -1235,15 +1248,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="D17" s="3">
         <v>2248</v>
@@ -1272,15 +1285,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D18" s="3">
         <v>2178</v>
@@ -1308,15 +1321,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="D19" s="3">
         <v>1489</v>
@@ -1345,15 +1358,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="D20" s="3">
         <v>2430</v>
@@ -1382,15 +1395,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="D21" s="3">
         <v>2230</v>
@@ -1419,15 +1432,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3">
         <v>1345</v>
@@ -1454,15 +1467,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3">
         <v>1725</v>
@@ -1489,15 +1502,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3">
         <v>995</v>
@@ -1524,15 +1537,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3">
         <v>1047</v>
@@ -1559,15 +1572,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D26" s="3">
         <v>558</v>
@@ -1594,15 +1607,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D27" s="3">
         <v>934</v>
@@ -1629,15 +1642,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D28" s="3">
         <v>977</v>
@@ -1664,15 +1677,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3">
         <v>1328</v>
@@ -1699,15 +1712,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D30" s="3">
         <v>1324</v>
@@ -1734,15 +1747,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3">
         <v>1000</v>
@@ -1769,15 +1782,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D32" s="3">
         <v>1257</v>
@@ -1804,15 +1817,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3">
         <v>1070</v>
@@ -1839,15 +1852,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D34" s="3">
         <v>1114</v>
@@ -1874,15 +1887,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D35" s="3">
         <v>1171</v>
@@ -1909,15 +1922,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D36" s="3">
         <v>1250</v>
@@ -1944,15 +1957,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D37" s="3">
         <v>1029</v>
@@ -1979,15 +1992,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D38" s="3">
         <v>1050</v>
@@ -2014,15 +2027,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D39" s="3">
         <v>1050</v>
@@ -2049,15 +2062,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D40" s="3">
         <v>974</v>
@@ -2084,15 +2097,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D41" s="3">
         <v>1172</v>
@@ -2119,15 +2132,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D42" s="3">
         <v>833</v>
@@ -2154,15 +2167,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D43" s="3">
         <v>1016</v>
@@ -2189,15 +2202,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D44" s="3">
         <v>997</v>
@@ -2224,15 +2237,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D45" s="3">
         <v>1688</v>

</xml_diff>